<commit_message>
Prueba con openpyxl realizada
</commit_message>
<xml_diff>
--- a/openpyxl-docs/prueba.xlsx
+++ b/openpyxl-docs/prueba.xlsx
@@ -1,44 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PauloV\Desktop\excelGenerator\openpyxl-docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE1EC21-4751-4974-8A6E-CD824F6C3511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12576" windowWidth="23256" xWindow="-108" yWindow="-108"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="hoja3" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="hoja1" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="hoja2" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Sheet" sheetId="2" r:id="rId1"/>
+    <sheet name="hoja1" sheetId="3" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -54,84 +57,25 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -419,78 +363,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="F19:F19"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="19">
-      <c r="F19" s="1" t="n"/>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F19" s="1"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
 </file>
</xml_diff>